<commit_message>
bug fixes for JIRA tickets LLR-210 and LLR-217
</commit_message>
<xml_diff>
--- a/app/docs/LLRbulkuploadformhelp.xlsx
+++ b/app/docs/LLRbulkuploadformhelp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dougie\Documents\llrep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dougie\Documents\projects\LLR-demo\app\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD2A37DD-F17C-44C7-A59C-1E1A43AB9789}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E5C5955-EAFD-4B4A-A47A-D1EF769C86BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LLRbulkuploadformhelp" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>LessonDateAdded</t>
   </si>
   <si>
-    <t>The date the lesson was identified or added to the repository</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -128,12 +125,15 @@
   </si>
   <si>
     <t>The lesson type; what went well (WWW) or even better if (EBI). Can also use lower case</t>
+  </si>
+  <si>
+    <t>The date the lesson was identified or added to the repository. Must be in the format dd/mm/yyyy or yyyy-mm-dd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -668,9 +668,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -678,6 +675,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1037,18 +1037,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
@@ -1061,7 +1061,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="5"/>
     </row>
@@ -1071,7 +1071,7 @@
     </row>
     <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1080,13 +1080,13 @@
     </row>
     <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4"/>
     </row>
@@ -1094,173 +1094,173 @@
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>26</v>
+      <c r="D8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>44145</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="D9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="8">
+        <v>23</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="9">
-        <v>23</v>
-      </c>
-      <c r="J9" s="9" t="s">
+      <c r="I10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K10" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="12" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" s="3"/>
@@ -1284,7 +1284,7 @@
     <mergeCell ref="B10:B15"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D14" r:id="rId1"/>
+    <hyperlink ref="D14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>